<commit_message>
Just settings on figures again
</commit_message>
<xml_diff>
--- a/output/sites/table_summary_sites_nut_total_estimates.xlsx
+++ b/output/sites/table_summary_sites_nut_total_estimates.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">scat_compo</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t xml:space="preserve">mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5% quantile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97.5% quantile</t>
   </si>
   <si>
     <t xml:space="preserve">min</t>
@@ -484,22 +490,22 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1.9571</v>
+        <v>2.1878</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2411</v>
+        <v>0.2586</v>
       </c>
       <c r="G3" t="n">
-        <v>0.106</v>
+        <v>0.1144</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0462</v>
+        <v>0.0515</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0178</v>
+        <v>0.0194</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0016</v>
+        <v>0.0018</v>
       </c>
     </row>
     <row r="4">
@@ -516,22 +522,22 @@
         <v>15</v>
       </c>
       <c r="E4" t="n">
-        <v>3.3615</v>
+        <v>3.1213</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3605</v>
+        <v>0.3466</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1754</v>
+        <v>0.1606</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0763</v>
+        <v>0.0719</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0285</v>
+        <v>0.0265</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0027</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="5">
@@ -542,28 +548,28 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" t="n">
-        <v>7.9221</v>
+        <v>1.9571</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9067</v>
+        <v>0.2411</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4125</v>
+        <v>0.106</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1848</v>
+        <v>0.0462</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0687</v>
+        <v>0.0178</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0064</v>
+        <v>0.0016</v>
       </c>
     </row>
     <row r="6">
@@ -574,28 +580,28 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" t="n">
-        <v>5.6126</v>
+        <v>3.3615</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7135</v>
+        <v>0.3605</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3213</v>
+        <v>0.1754</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1354</v>
+        <v>0.0763</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0539</v>
+        <v>0.0285</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0047</v>
+        <v>0.0027</v>
       </c>
     </row>
     <row r="7">
@@ -606,28 +612,28 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" t="n">
-        <v>9.9626</v>
+        <v>7.9221</v>
       </c>
       <c r="F7" t="n">
-        <v>1.0745</v>
+        <v>0.9067</v>
       </c>
       <c r="G7" t="n">
-        <v>0.522</v>
+        <v>0.4125</v>
       </c>
       <c r="H7" t="n">
-        <v>0.233</v>
+        <v>0.1848</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0841</v>
+        <v>0.0687</v>
       </c>
       <c r="J7" t="n">
-        <v>0.008</v>
+        <v>0.0064</v>
       </c>
     </row>
     <row r="8">
@@ -638,28 +644,28 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10.5633</v>
+        <v>6.567</v>
       </c>
       <c r="F8" t="n">
-        <v>1.2091</v>
+        <v>0.7768</v>
       </c>
       <c r="G8" t="n">
-        <v>0.55</v>
+        <v>0.3451</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2464</v>
+        <v>0.1546</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0916</v>
+        <v>0.0585</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0086</v>
+        <v>0.0054</v>
       </c>
     </row>
     <row r="9">
@@ -670,28 +676,28 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" t="n">
-        <v>7.5697</v>
+        <v>9.3249</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9546</v>
+        <v>1.0385</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4276</v>
+        <v>0.4805</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1817</v>
+        <v>0.2157</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0718</v>
+        <v>0.0798</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0063</v>
+        <v>0.0075</v>
       </c>
     </row>
     <row r="10">
@@ -702,28 +708,28 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" t="n">
-        <v>13.2454</v>
+        <v>5.6126</v>
       </c>
       <c r="F10" t="n">
-        <v>1.429</v>
+        <v>0.7135</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6974</v>
+        <v>0.3213</v>
       </c>
       <c r="H10" t="n">
-        <v>0.3088</v>
+        <v>0.1354</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1126</v>
+        <v>0.0539</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0107</v>
+        <v>0.0047</v>
       </c>
     </row>
     <row r="11">
@@ -734,28 +740,28 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>25</v>
+        <v>9.9626</v>
       </c>
       <c r="F11" t="n">
-        <v>25</v>
+        <v>1.0745</v>
       </c>
       <c r="G11" t="n">
-        <v>25</v>
+        <v>0.522</v>
       </c>
       <c r="H11" t="n">
-        <v>25</v>
+        <v>0.233</v>
       </c>
       <c r="I11" t="n">
-        <v>25</v>
+        <v>0.0841</v>
       </c>
       <c r="J11" t="n">
-        <v>24</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="12">
@@ -766,28 +772,28 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E12" t="n">
-        <v>75</v>
+        <v>10.5633</v>
       </c>
       <c r="F12" t="n">
-        <v>75</v>
+        <v>1.2091</v>
       </c>
       <c r="G12" t="n">
-        <v>75</v>
+        <v>0.55</v>
       </c>
       <c r="H12" t="n">
-        <v>75</v>
+        <v>0.2464</v>
       </c>
       <c r="I12" t="n">
-        <v>75</v>
+        <v>0.0916</v>
       </c>
       <c r="J12" t="n">
-        <v>74</v>
+        <v>0.0086</v>
       </c>
     </row>
     <row r="13">
@@ -795,31 +801,31 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3.0726</v>
+        <v>8.7627</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3516</v>
+        <v>1.0383</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1596</v>
+        <v>0.4609</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0717</v>
+        <v>0.2061</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0266</v>
+        <v>0.0779</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0025</v>
+        <v>0.0072</v>
       </c>
     </row>
     <row r="14">
@@ -827,31 +833,31 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" t="n">
-        <v>2.4749</v>
+        <v>12.4136</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3185</v>
+        <v>1.3827</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1345</v>
+        <v>0.6422</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0602</v>
+        <v>0.2868</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0235</v>
+        <v>0.1061</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0021</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15">
@@ -859,31 +865,31 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E15" t="n">
-        <v>3.5971</v>
+        <v>7.5697</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3905</v>
+        <v>0.9546</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1836</v>
+        <v>0.4276</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0845</v>
+        <v>0.1817</v>
       </c>
       <c r="I15" t="n">
-        <v>0.03</v>
+        <v>0.0718</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0029</v>
+        <v>0.0063</v>
       </c>
     </row>
     <row r="16">
@@ -891,31 +897,31 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>9.2187</v>
+        <v>13.2454</v>
       </c>
       <c r="F16" t="n">
-        <v>1.0547</v>
+        <v>1.429</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4788</v>
+        <v>0.6974</v>
       </c>
       <c r="H16" t="n">
-        <v>0.2153</v>
+        <v>0.3088</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0798</v>
+        <v>0.1126</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0075</v>
+        <v>0.0107</v>
       </c>
     </row>
     <row r="17">
@@ -923,31 +929,31 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E17" t="n">
-        <v>7.4963</v>
+        <v>25</v>
       </c>
       <c r="F17" t="n">
-        <v>0.968</v>
+        <v>25</v>
       </c>
       <c r="G17" t="n">
-        <v>0.4052</v>
+        <v>25</v>
       </c>
       <c r="H17" t="n">
-        <v>0.1794</v>
+        <v>25</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0702</v>
+        <v>25</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0063</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
@@ -955,31 +961,31 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E18" t="n">
-        <v>11.0216</v>
+        <v>75</v>
       </c>
       <c r="F18" t="n">
-        <v>1.1604</v>
+        <v>75</v>
       </c>
       <c r="G18" t="n">
-        <v>0.5601</v>
+        <v>75</v>
       </c>
       <c r="H18" t="n">
-        <v>0.2559</v>
+        <v>75</v>
       </c>
       <c r="I18" t="n">
-        <v>0.092</v>
+        <v>75</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0089</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19">
@@ -987,31 +993,31 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
       <c r="E19" t="n">
-        <v>12.2914</v>
+        <v>3.0726</v>
       </c>
       <c r="F19" t="n">
-        <v>1.4063</v>
+        <v>0.3516</v>
       </c>
       <c r="G19" t="n">
-        <v>0.6385</v>
+        <v>0.1596</v>
       </c>
       <c r="H19" t="n">
-        <v>0.287</v>
+        <v>0.0717</v>
       </c>
       <c r="I19" t="n">
-        <v>0.1064</v>
+        <v>0.0266</v>
       </c>
       <c r="J19" t="n">
-        <v>0.01</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="20">
@@ -1019,31 +1025,31 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
       </c>
       <c r="E20" t="n">
-        <v>9.9712</v>
+        <v>2.7216</v>
       </c>
       <c r="F20" t="n">
-        <v>1.2865</v>
+        <v>0.3297</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5398</v>
+        <v>0.1447</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2395</v>
+        <v>0.0649</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0937</v>
+        <v>0.0245</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0084</v>
+        <v>0.0022</v>
       </c>
     </row>
     <row r="21">
@@ -1051,31 +1057,31 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21" t="n">
-        <v>14.6188</v>
+        <v>3.4302</v>
       </c>
       <c r="F21" t="n">
-        <v>1.5489</v>
+        <v>0.3735</v>
       </c>
       <c r="G21" t="n">
-        <v>0.7395</v>
+        <v>0.1749</v>
       </c>
       <c r="H21" t="n">
-        <v>0.3404</v>
+        <v>0.0789</v>
       </c>
       <c r="I21" t="n">
-        <v>0.1211</v>
+        <v>0.0288</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0119</v>
+        <v>0.0028</v>
       </c>
     </row>
     <row r="22">
@@ -1083,31 +1089,31 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22" t="n">
-        <v>25</v>
+        <v>2.4749</v>
       </c>
       <c r="F22" t="n">
-        <v>25</v>
+        <v>0.3185</v>
       </c>
       <c r="G22" t="n">
-        <v>25</v>
+        <v>0.1345</v>
       </c>
       <c r="H22" t="n">
-        <v>25</v>
+        <v>0.0602</v>
       </c>
       <c r="I22" t="n">
-        <v>25</v>
+        <v>0.0235</v>
       </c>
       <c r="J22" t="n">
-        <v>25</v>
+        <v>0.0021</v>
       </c>
     </row>
     <row r="23">
@@ -1115,252 +1121,252 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" t="n">
-        <v>75</v>
+        <v>3.5971</v>
       </c>
       <c r="F23" t="n">
-        <v>75</v>
+        <v>0.3905</v>
       </c>
       <c r="G23" t="n">
-        <v>75</v>
+        <v>0.1836</v>
       </c>
       <c r="H23" t="n">
-        <v>75</v>
+        <v>0.0845</v>
       </c>
       <c r="I23" t="n">
-        <v>75</v>
+        <v>0.03</v>
       </c>
       <c r="J23" t="n">
-        <v>75</v>
+        <v>0.0029</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
       <c r="E24" t="n">
-        <v>2.7733</v>
+        <v>9.2187</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3481</v>
+        <v>1.0547</v>
       </c>
       <c r="G24" t="n">
-        <v>0.1997</v>
+        <v>0.4788</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0533</v>
+        <v>0.2153</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0282</v>
+        <v>0.0798</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0023</v>
+        <v>0.0075</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
       <c r="E25" t="n">
-        <v>2.0192</v>
+        <v>8.213</v>
       </c>
       <c r="F25" t="n">
-        <v>0.281</v>
+        <v>0.9893</v>
       </c>
       <c r="G25" t="n">
-        <v>0.1602</v>
+        <v>0.4361</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0414</v>
+        <v>0.1957</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0227</v>
+        <v>0.0737</v>
       </c>
       <c r="J25" t="n">
-        <v>0.0017</v>
+        <v>0.0068</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
       <c r="E26" t="n">
-        <v>3.6713</v>
+        <v>10.2298</v>
       </c>
       <c r="F26" t="n">
-        <v>0.4171</v>
+        <v>1.1194</v>
       </c>
       <c r="G26" t="n">
-        <v>0.2465</v>
+        <v>0.525</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0653</v>
+        <v>0.2349</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0353</v>
+        <v>0.0856</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0029</v>
+        <v>0.0083</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
         <v>16</v>
       </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
       <c r="E27" t="n">
-        <v>8.319</v>
+        <v>7.4963</v>
       </c>
       <c r="F27" t="n">
-        <v>1.044</v>
+        <v>0.968</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5993</v>
+        <v>0.4052</v>
       </c>
       <c r="H27" t="n">
-        <v>0.1597</v>
+        <v>0.1794</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0846</v>
+        <v>0.0702</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0068</v>
+        <v>0.0063</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E28" t="n">
-        <v>6.1881</v>
+        <v>11.0216</v>
       </c>
       <c r="F28" t="n">
-        <v>0.8502</v>
+        <v>1.1604</v>
       </c>
       <c r="G28" t="n">
-        <v>0.4822</v>
+        <v>0.5601</v>
       </c>
       <c r="H28" t="n">
-        <v>0.1235</v>
+        <v>0.2559</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0672</v>
+        <v>0.092</v>
       </c>
       <c r="J28" t="n">
-        <v>0.0051</v>
+        <v>0.0089</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E29" t="n">
-        <v>10.5414</v>
+        <v>12.2914</v>
       </c>
       <c r="F29" t="n">
-        <v>1.2539</v>
+        <v>1.4063</v>
       </c>
       <c r="G29" t="n">
-        <v>0.749</v>
+        <v>0.6385</v>
       </c>
       <c r="H29" t="n">
-        <v>0.193</v>
+        <v>0.287</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1048</v>
+        <v>0.1064</v>
       </c>
       <c r="J29" t="n">
-        <v>0.0084</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E30" t="n">
-        <v>11.0923</v>
+        <v>10.9707</v>
       </c>
       <c r="F30" t="n">
-        <v>1.3921</v>
+        <v>1.3228</v>
       </c>
       <c r="G30" t="n">
-        <v>0.7991</v>
+        <v>0.5807</v>
       </c>
       <c r="H30" t="n">
-        <v>0.213</v>
+        <v>0.2607</v>
       </c>
       <c r="I30" t="n">
-        <v>0.1128</v>
+        <v>0.0982</v>
       </c>
       <c r="J30" t="n">
         <v>0.009</v>
@@ -1368,481 +1374,1249 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E31" t="n">
-        <v>8.2303</v>
+        <v>13.6369</v>
       </c>
       <c r="F31" t="n">
-        <v>1.1312</v>
+        <v>1.4883</v>
       </c>
       <c r="G31" t="n">
-        <v>0.6424</v>
+        <v>0.6984</v>
       </c>
       <c r="H31" t="n">
-        <v>0.1654</v>
+        <v>0.3133</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0903</v>
+        <v>0.1142</v>
       </c>
       <c r="J31" t="n">
-        <v>0.0068</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E32" t="n">
-        <v>14.0999</v>
+        <v>9.9712</v>
       </c>
       <c r="F32" t="n">
-        <v>1.6648</v>
+        <v>1.2865</v>
       </c>
       <c r="G32" t="n">
-        <v>0.9914</v>
+        <v>0.5398</v>
       </c>
       <c r="H32" t="n">
-        <v>0.2574</v>
+        <v>0.2395</v>
       </c>
       <c r="I32" t="n">
-        <v>0.14</v>
+        <v>0.0937</v>
       </c>
       <c r="J32" t="n">
-        <v>0.0112</v>
+        <v>0.0084</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E33" t="n">
-        <v>25</v>
+        <v>14.6188</v>
       </c>
       <c r="F33" t="n">
-        <v>25</v>
+        <v>1.5489</v>
       </c>
       <c r="G33" t="n">
-        <v>25</v>
+        <v>0.7395</v>
       </c>
       <c r="H33" t="n">
-        <v>25</v>
+        <v>0.3404</v>
       </c>
       <c r="I33" t="n">
-        <v>25</v>
+        <v>0.1211</v>
       </c>
       <c r="J33" t="n">
-        <v>26</v>
+        <v>0.0119</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
         <v>20</v>
       </c>
-      <c r="B34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" t="s">
-        <v>18</v>
-      </c>
       <c r="E34" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="F34" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="G34" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="H34" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="I34" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="J34" t="n">
-        <v>76</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
         <v>20</v>
       </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" t="s">
-        <v>13</v>
-      </c>
       <c r="E35" t="n">
-        <v>2.92</v>
+        <v>75</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3013</v>
+        <v>75</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0922</v>
+        <v>75</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0807</v>
+        <v>75</v>
       </c>
       <c r="I35" t="n">
-        <v>0.0208</v>
+        <v>75</v>
       </c>
       <c r="J35" t="n">
-        <v>0.0024</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E36" t="n">
-        <v>2.376</v>
+        <v>2.7733</v>
       </c>
       <c r="F36" t="n">
-        <v>0.2735</v>
+        <v>0.3481</v>
       </c>
       <c r="G36" t="n">
-        <v>0.0814</v>
+        <v>0.1997</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0658</v>
+        <v>0.0533</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0185</v>
+        <v>0.0282</v>
       </c>
       <c r="J36" t="n">
-        <v>0.002</v>
+        <v>0.0023</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" t="n">
-        <v>3.5952</v>
+        <v>2.2748</v>
       </c>
       <c r="F37" t="n">
-        <v>0.3321</v>
+        <v>0.2978</v>
       </c>
       <c r="G37" t="n">
-        <v>0.1078</v>
+        <v>0.1687</v>
       </c>
       <c r="H37" t="n">
-        <v>0.0984</v>
+        <v>0.0448</v>
       </c>
       <c r="I37" t="n">
-        <v>0.0236</v>
+        <v>0.0238</v>
       </c>
       <c r="J37" t="n">
-        <v>0.0029</v>
+        <v>0.0019</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E38" t="n">
-        <v>8.7663</v>
+        <v>3.2722</v>
       </c>
       <c r="F38" t="n">
-        <v>0.9039</v>
+        <v>0.3977</v>
       </c>
       <c r="G38" t="n">
-        <v>0.2768</v>
+        <v>0.2304</v>
       </c>
       <c r="H38" t="n">
-        <v>0.2422</v>
+        <v>0.0617</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0625</v>
+        <v>0.0325</v>
       </c>
       <c r="J38" t="n">
-        <v>0.0071</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
         <v>16</v>
       </c>
-      <c r="D39" t="s">
-        <v>14</v>
-      </c>
       <c r="E39" t="n">
-        <v>7.2627</v>
+        <v>2.0192</v>
       </c>
       <c r="F39" t="n">
-        <v>0.8206</v>
+        <v>0.281</v>
       </c>
       <c r="G39" t="n">
-        <v>0.2416</v>
+        <v>0.1602</v>
       </c>
       <c r="H39" t="n">
-        <v>0.1998</v>
+        <v>0.0414</v>
       </c>
       <c r="I39" t="n">
-        <v>0.055</v>
+        <v>0.0227</v>
       </c>
       <c r="J39" t="n">
-        <v>0.006</v>
+        <v>0.0017</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E40" t="n">
-        <v>10.7596</v>
+        <v>3.6713</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9937</v>
+        <v>0.4171</v>
       </c>
       <c r="G40" t="n">
-        <v>0.3187</v>
+        <v>0.2465</v>
       </c>
       <c r="H40" t="n">
-        <v>0.2928</v>
+        <v>0.0653</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0701</v>
+        <v>0.0353</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0086</v>
+        <v>0.0029</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
       </c>
       <c r="E41" t="n">
-        <v>11.6863</v>
+        <v>8.319</v>
       </c>
       <c r="F41" t="n">
-        <v>1.2053</v>
+        <v>1.044</v>
       </c>
       <c r="G41" t="n">
-        <v>0.369</v>
+        <v>0.5993</v>
       </c>
       <c r="H41" t="n">
-        <v>0.3229</v>
+        <v>0.1597</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0833</v>
+        <v>0.0846</v>
       </c>
       <c r="J41" t="n">
-        <v>0.0095</v>
+        <v>0.0068</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
       </c>
       <c r="E42" t="n">
-        <v>9.6991</v>
+        <v>6.8152</v>
       </c>
       <c r="F42" t="n">
-        <v>1.1</v>
+        <v>0.8987</v>
       </c>
       <c r="G42" t="n">
-        <v>0.3238</v>
+        <v>0.5057</v>
       </c>
       <c r="H42" t="n">
-        <v>0.2656</v>
+        <v>0.1344</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0737</v>
+        <v>0.0717</v>
       </c>
       <c r="J42" t="n">
-        <v>0.008</v>
+        <v>0.0056</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
         <v>15</v>
       </c>
       <c r="E43" t="n">
-        <v>14.2913</v>
+        <v>9.7561</v>
       </c>
       <c r="F43" t="n">
-        <v>1.3253</v>
+        <v>1.1867</v>
       </c>
       <c r="G43" t="n">
-        <v>0.4261</v>
+        <v>0.6965</v>
       </c>
       <c r="H43" t="n">
-        <v>0.3878</v>
+        <v>0.1854</v>
       </c>
       <c r="I43" t="n">
-        <v>0.0935</v>
+        <v>0.0983</v>
       </c>
       <c r="J43" t="n">
-        <v>0.0114</v>
+        <v>0.0079</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E44" t="n">
-        <v>25</v>
+        <v>6.1881</v>
       </c>
       <c r="F44" t="n">
-        <v>25</v>
+        <v>0.8502</v>
       </c>
       <c r="G44" t="n">
-        <v>25</v>
+        <v>0.4822</v>
       </c>
       <c r="H44" t="n">
-        <v>25</v>
+        <v>0.1235</v>
       </c>
       <c r="I44" t="n">
-        <v>25</v>
+        <v>0.0672</v>
       </c>
       <c r="J44" t="n">
-        <v>25</v>
+        <v>0.0051</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="n">
+        <v>10.5414</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1.2539</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.749</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.193</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.1048</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.0084</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" t="n">
+        <v>11.0923</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1.3921</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.7991</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.213</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.1128</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.009</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" t="n">
+        <v>9.1051</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1.1967</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.6761</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.1793</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.0956</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.0075</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" t="n">
+        <v>13.0311</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1.5845</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.9245</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.2468</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.1306</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.0105</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" t="n">
+        <v>8.2303</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1.1312</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.6424</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.1654</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.0903</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.0068</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="n">
+        <v>14.0999</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1.6648</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.9914</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.2574</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.0112</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
         <v>20</v>
       </c>
-      <c r="B45" t="s">
+      <c r="E51" t="n">
+        <v>25</v>
+      </c>
+      <c r="F51" t="n">
+        <v>25</v>
+      </c>
+      <c r="G51" t="n">
+        <v>25</v>
+      </c>
+      <c r="H51" t="n">
+        <v>25</v>
+      </c>
+      <c r="I51" t="n">
+        <v>25</v>
+      </c>
+      <c r="J51" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" t="n">
+        <v>75</v>
+      </c>
+      <c r="F52" t="n">
+        <v>75</v>
+      </c>
+      <c r="G52" t="n">
+        <v>75</v>
+      </c>
+      <c r="H52" t="n">
+        <v>75</v>
+      </c>
+      <c r="I52" t="n">
+        <v>75</v>
+      </c>
+      <c r="J52" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.3013</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.0922</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.0807</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.0208</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.0024</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2.5979</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.2819</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.0839</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.0721</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.0194</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.0021</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.259</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.3202</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.1012</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.0901</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.0225</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.0026</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2.376</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.2735</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.0814</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.0658</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.0185</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.5952</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.3321</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.1078</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.0984</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.0236</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.0029</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" t="n">
+        <v>8.7663</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.9039</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.2768</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.2422</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.0071</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" t="n">
+        <v>7.7745</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.8487</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.2527</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.2162</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.0582</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.0064</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" t="n">
+        <v>9.7448</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.9594</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.3018</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.2681</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.0671</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.0079</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" t="n">
+        <v>7.2627</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.8206</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.2416</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.1998</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" t="n">
+        <v>10.7596</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.9937</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.3187</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.2928</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.0701</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.0086</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" t="s">
         <v>19</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" t="n">
+        <v>11.6863</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1.2053</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.369</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.3229</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.0833</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.0095</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" t="n">
+        <v>10.3848</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1.1334</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.3366</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.2893</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.0777</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" t="n">
+        <v>12.9893</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1.2773</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.4021</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.3581</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.0895</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.0105</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>19</v>
+      </c>
+      <c r="D66" t="s">
         <v>16</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E66" t="n">
+        <v>9.6991</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.3238</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.2656</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.0737</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" t="n">
+        <v>14.2913</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1.3253</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.4261</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.3878</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.0935</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.0114</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" t="n">
+        <v>25</v>
+      </c>
+      <c r="F68" t="n">
+        <v>25</v>
+      </c>
+      <c r="G68" t="n">
+        <v>25</v>
+      </c>
+      <c r="H68" t="n">
+        <v>25</v>
+      </c>
+      <c r="I68" t="n">
+        <v>25</v>
+      </c>
+      <c r="J68" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" t="s">
         <v>18</v>
       </c>
-      <c r="E45" t="n">
+      <c r="D69" t="s">
+        <v>20</v>
+      </c>
+      <c r="E69" t="n">
         <v>75</v>
       </c>
-      <c r="F45" t="n">
+      <c r="F69" t="n">
         <v>75</v>
       </c>
-      <c r="G45" t="n">
+      <c r="G69" t="n">
         <v>75</v>
       </c>
-      <c r="H45" t="n">
+      <c r="H69" t="n">
         <v>75</v>
       </c>
-      <c r="I45" t="n">
+      <c r="I69" t="n">
         <v>75</v>
       </c>
-      <c r="J45" t="n">
+      <c r="J69" t="n">
         <v>75</v>
       </c>
     </row>

</xml_diff>